<commit_message>
revise freq of data
</commit_message>
<xml_diff>
--- a/test/testdata1.xlsx
+++ b/test/testdata1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vertices" sheetId="1" state="visible" r:id="rId2"/>
@@ -1033,11 +1033,11 @@
   </sheetPr>
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.42"/>
@@ -3091,11 +3091,11 @@
   </sheetPr>
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E82" activeCellId="0" sqref="E82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
@@ -3185,7 +3185,7 @@
         <v>77</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>78</v>
@@ -3248,7 +3248,7 @@
         <v>77</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>80</v>
@@ -3311,7 +3311,7 @@
         <v>77</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>80</v>
@@ -3374,7 +3374,7 @@
         <v>77</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>83</v>
@@ -3437,7 +3437,7 @@
         <v>77</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>85</v>
@@ -3500,7 +3500,7 @@
         <v>77</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>85</v>
@@ -3563,7 +3563,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>88</v>
@@ -3626,7 +3626,7 @@
         <v>77</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>88</v>
@@ -3689,7 +3689,7 @@
         <v>77</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>85</v>
@@ -3752,7 +3752,7 @@
         <v>77</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>92</v>
@@ -3815,7 +3815,7 @@
         <v>77</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>85</v>
@@ -3878,7 +3878,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>95</v>
@@ -3941,7 +3941,7 @@
         <v>77</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>85</v>
@@ -4004,7 +4004,7 @@
         <v>77</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>98</v>
@@ -4067,7 +4067,7 @@
         <v>77</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>88</v>
@@ -4130,7 +4130,7 @@
         <v>77</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>101</v>
@@ -4193,7 +4193,7 @@
         <v>77</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>101</v>
@@ -4256,7 +4256,7 @@
         <v>77</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>104</v>
@@ -4319,7 +4319,7 @@
         <v>77</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>106</v>
@@ -4382,7 +4382,7 @@
         <v>77</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>108</v>
@@ -4445,7 +4445,7 @@
         <v>77</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>110</v>
@@ -4508,7 +4508,7 @@
         <v>77</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>112</v>
@@ -4571,7 +4571,7 @@
         <v>77</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>106</v>
@@ -4634,7 +4634,7 @@
         <v>77</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>115</v>
@@ -4697,7 +4697,7 @@
         <v>77</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>117</v>
@@ -4760,7 +4760,7 @@
         <v>77</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>119</v>
@@ -4823,7 +4823,7 @@
         <v>77</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>121</v>
@@ -4886,7 +4886,7 @@
         <v>77</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>123</v>
@@ -4949,7 +4949,7 @@
         <v>77</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>125</v>
@@ -5012,7 +5012,7 @@
         <v>77</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>127</v>
@@ -5075,7 +5075,7 @@
         <v>77</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>129</v>
@@ -5138,7 +5138,7 @@
         <v>77</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>131</v>
@@ -5201,7 +5201,7 @@
         <v>77</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>133</v>
@@ -5264,7 +5264,7 @@
         <v>77</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>129</v>
@@ -5327,7 +5327,7 @@
         <v>77</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>136</v>
@@ -5390,7 +5390,7 @@
         <v>77</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>138</v>
@@ -5453,7 +5453,7 @@
         <v>77</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>140</v>
@@ -5516,7 +5516,7 @@
         <v>77</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>142</v>
@@ -5579,7 +5579,7 @@
         <v>77</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>106</v>
@@ -5642,7 +5642,7 @@
         <v>77</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>106</v>
@@ -5705,7 +5705,7 @@
         <v>77</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>106</v>
@@ -5768,7 +5768,7 @@
         <v>77</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>147</v>
@@ -5831,7 +5831,7 @@
         <v>77</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>149</v>
@@ -5894,7 +5894,7 @@
         <v>77</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>151</v>
@@ -5957,7 +5957,7 @@
         <v>77</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>153</v>
@@ -6020,7 +6020,7 @@
         <v>77</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>151</v>
@@ -6083,7 +6083,7 @@
         <v>77</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>156</v>
@@ -6146,7 +6146,7 @@
         <v>77</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>158</v>
@@ -6209,7 +6209,7 @@
         <v>77</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" s="0" t="s">
         <v>160</v>
@@ -6272,7 +6272,7 @@
         <v>77</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>162</v>
@@ -6335,7 +6335,7 @@
         <v>77</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>164</v>
@@ -6398,7 +6398,7 @@
         <v>77</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>166</v>
@@ -6461,7 +6461,7 @@
         <v>77</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>168</v>
@@ -6524,7 +6524,7 @@
         <v>77</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>166</v>
@@ -6587,7 +6587,7 @@
         <v>77</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>166</v>
@@ -6650,7 +6650,7 @@
         <v>77</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>172</v>
@@ -6713,7 +6713,7 @@
         <v>77</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>174</v>
@@ -6776,7 +6776,7 @@
         <v>77</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" s="0" t="s">
         <v>176</v>
@@ -6839,7 +6839,7 @@
         <v>77</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>178</v>
@@ -6902,7 +6902,7 @@
         <v>77</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>180</v>
@@ -6965,7 +6965,7 @@
         <v>77</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>182</v>
@@ -7028,7 +7028,7 @@
         <v>77</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>184</v>
@@ -7091,7 +7091,7 @@
         <v>77</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>186</v>
@@ -8288,7 +8288,7 @@
         <v>222</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>223</v>
@@ -8351,7 +8351,7 @@
         <v>222</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>225</v>
@@ -8414,7 +8414,7 @@
         <v>222</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>227</v>
@@ -8491,7 +8491,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8528,13 +8528,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.13"/>
@@ -10471,6 +10471,7 @@
         <v>18189</v>
       </c>
     </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
test data revision for 3 and 4
</commit_message>
<xml_diff>
--- a/test/testdata1.xlsx
+++ b/test/testdata1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vertices" sheetId="1" state="visible" r:id="rId2"/>
@@ -1033,11 +1033,11 @@
   </sheetPr>
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.42"/>
@@ -3091,17 +3091,17 @@
   </sheetPr>
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E82" activeCellId="0" sqref="E82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="65.07"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.01"/>
@@ -8491,7 +8491,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8530,11 +8530,11 @@
   </sheetPr>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.13"/>

</xml_diff>